<commit_message>
Adiciona alterações no arquivo cronograma
</commit_message>
<xml_diff>
--- a/Quarto Semestre/Projeto_Integrador/Quarta Entrega/Cronograma.xlsx
+++ b/Quarto Semestre/Projeto_Integrador/Quarta Entrega/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richa\OneDrive\Área de Trabalho\Faculdade\Quarto Semestre\Projeto_Integrador\Quarta Entrega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7190FF0E-46EE-484E-AC2D-886B0241195C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4593375F-FCB5-468A-A1F4-94EE908B2812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E13B2B5E-4C2D-4D8A-B3E2-CD058EB1906D}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Cronograma</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Descrição da Atividade</t>
   </si>
@@ -56,49 +53,124 @@
     <t>Fim</t>
   </si>
   <si>
-    <t>Identificador de Atividade</t>
-  </si>
-  <si>
-    <t>ATV 01</t>
-  </si>
-  <si>
-    <t>ATV 02</t>
-  </si>
-  <si>
-    <t>ATV 03</t>
-  </si>
-  <si>
-    <t>ATV 04</t>
-  </si>
-  <si>
-    <t>ATV 05</t>
-  </si>
-  <si>
-    <t>ATV 06</t>
-  </si>
-  <si>
-    <t>Definição da carga horária</t>
-  </si>
-  <si>
-    <t>Preparação do material de apoio</t>
-  </si>
-  <si>
-    <t>Elaboração de ementa</t>
-  </si>
-  <si>
-    <t>Treinamento dos instrutores</t>
-  </si>
-  <si>
-    <t>Divisão de turmas por instrutores</t>
-  </si>
-  <si>
-    <t>Execução do curso</t>
-  </si>
-  <si>
-    <t>ATV 07</t>
-  </si>
-  <si>
-    <t>Site para documentação/material de apoio</t>
+    <t>Identificador de Requisito</t>
+  </si>
+  <si>
+    <t>RE 8</t>
+  </si>
+  <si>
+    <t>RE 2</t>
+  </si>
+  <si>
+    <t>RE 3</t>
+  </si>
+  <si>
+    <t>Elaboração da ementa</t>
+  </si>
+  <si>
+    <t>Cronograma Ementa e Preparação</t>
+  </si>
+  <si>
+    <t>Definição do conteúdo programático</t>
+  </si>
+  <si>
+    <t>Definição da metodologia</t>
+  </si>
+  <si>
+    <t>RE 4</t>
+  </si>
+  <si>
+    <t>Definição do método de avaliação</t>
+  </si>
+  <si>
+    <t>RE 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Definição da carga horária e Escolha de uma linguagem adequada</t>
+  </si>
+  <si>
+    <t>RE 1/RE 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Definição de referências</t>
+  </si>
+  <si>
+    <t>RE 7</t>
+  </si>
+  <si>
+    <t>Aprovação do plano de ensino</t>
+  </si>
+  <si>
+    <t>RE 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Processo de alteração</t>
+  </si>
+  <si>
+    <t>RE 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adaptação ao público-alvo</t>
+  </si>
+  <si>
+    <t>RE 12/RE 13</t>
+  </si>
+  <si>
+    <t>Limite de participantes e Garantia Máquina</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Fase de Execução do projeto</t>
+  </si>
+  <si>
+    <t>Cronograma Desenvolvimento Site</t>
+  </si>
+  <si>
+    <t>RS 1</t>
+  </si>
+  <si>
+    <t>Definição da estrutura e layout do site</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da Página Inicial (Home) com informações do projeto</t>
+  </si>
+  <si>
+    <t>Implementação da seção de Materiais Complementares</t>
+  </si>
+  <si>
+    <t>RS 2</t>
+  </si>
+  <si>
+    <t>Garantir que o site tenha uma Navegação Intuitiva</t>
+  </si>
+  <si>
+    <t>RS 3</t>
+  </si>
+  <si>
+    <t>RS 4</t>
+  </si>
+  <si>
+    <t>Garantir a Acessibilidade do site a pessoas com deficiências</t>
+  </si>
+  <si>
+    <t>RS 5</t>
+  </si>
+  <si>
+    <t>Garantir um Design Responsivo para funcionamento em diversos dispositivos</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da Área para Envio de Atividades e integração</t>
+  </si>
+  <si>
+    <t>RS 6</t>
+  </si>
+  <si>
+    <t>Realização de testes para verificar a funcionalidade e o design do site</t>
+  </si>
+  <si>
+    <t>Ajustes finais e otimizações no site</t>
   </si>
 </sst>
 </file>
@@ -233,6 +305,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -246,12 +324,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -574,48 +646,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00196F21-3F75-4841-AD7B-9DD04B193557}">
-  <dimension ref="B2:N12"/>
+  <dimension ref="B2:N31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:H6"/>
+      <selection activeCell="G11" sqref="G11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="4" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
@@ -625,195 +697,669 @@
       <c r="F5" s="11"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="6">
+      <c r="I6" s="8">
         <v>45200</v>
       </c>
-      <c r="J6" s="7"/>
+      <c r="J6" s="9"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="6">
-        <v>45200</v>
-      </c>
-      <c r="M6" s="7"/>
+      <c r="L6" s="8">
+        <v>45201</v>
+      </c>
+      <c r="M6" s="9"/>
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="6">
-        <v>45201</v>
-      </c>
-      <c r="J7" s="7"/>
+      <c r="I7" s="8">
+        <v>45202</v>
+      </c>
+      <c r="J7" s="9"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="6">
-        <v>45209</v>
-      </c>
-      <c r="M7" s="7"/>
+      <c r="L7" s="8">
+        <v>45204</v>
+      </c>
+      <c r="M7" s="9"/>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="2"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="6">
-        <v>45210</v>
-      </c>
-      <c r="J8" s="7"/>
+      <c r="I8" s="8">
+        <v>45205</v>
+      </c>
+      <c r="J8" s="9"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="6">
-        <v>45218</v>
-      </c>
-      <c r="M8" s="7"/>
+      <c r="L8" s="8">
+        <v>45208</v>
+      </c>
+      <c r="M8" s="9"/>
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="E9" s="9"/>
       <c r="F9" s="2"/>
       <c r="G9" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="6">
-        <v>45219</v>
-      </c>
-      <c r="J9" s="7"/>
+      <c r="I9" s="8">
+        <v>45209</v>
+      </c>
+      <c r="J9" s="9"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="6">
-        <v>45225</v>
-      </c>
-      <c r="M9" s="7"/>
+      <c r="L9" s="8">
+        <v>45213</v>
+      </c>
+      <c r="M9" s="9"/>
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="6">
-        <v>45226</v>
-      </c>
-      <c r="J10" s="7"/>
+      <c r="I10" s="8">
+        <v>45214</v>
+      </c>
+      <c r="J10" s="9"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="6">
-        <v>45227</v>
-      </c>
-      <c r="M10" s="7"/>
+      <c r="L10" s="8">
+        <v>45217</v>
+      </c>
+      <c r="M10" s="9"/>
       <c r="N10" s="2"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="6">
-        <v>45231</v>
-      </c>
-      <c r="J11" s="7"/>
+      <c r="I11" s="8">
+        <v>45218</v>
+      </c>
+      <c r="J11" s="9"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="6">
-        <v>45250</v>
-      </c>
-      <c r="M11" s="7"/>
+      <c r="L11" s="8">
+        <v>45220</v>
+      </c>
+      <c r="M11" s="9"/>
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="8">
+        <v>45221</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="8">
+        <v>45223</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="1">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="8">
+        <v>45224</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="8">
+        <v>45225</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="8">
+        <v>45226</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="8">
+        <v>45228</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="8">
+        <v>45229</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="8">
+        <v>45230</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="1">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="8">
+        <v>45231</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="8">
+        <v>45260</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="19" spans="2:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="21" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="6">
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="1">
+        <v>4</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="8">
         <v>45200</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="6">
+      <c r="J23" s="9"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="8">
+        <v>45203</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="1">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="8">
+        <v>45204</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="8">
+        <v>45208</v>
+      </c>
+      <c r="M24" s="9"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="1">
+        <v>4</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="8">
+        <v>45209</v>
+      </c>
+      <c r="J25" s="9"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="8">
+        <v>45212</v>
+      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="1">
+        <v>3</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="8">
+        <v>45213</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="8">
+        <v>45215</v>
+      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="1">
+        <v>3</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="8">
+        <v>45216</v>
+      </c>
+      <c r="J27" s="9"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="8">
+        <v>45218</v>
+      </c>
+      <c r="M27" s="9"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="1">
+        <v>3</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="8">
+        <v>45219</v>
+      </c>
+      <c r="J28" s="9"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="8">
+        <v>45221</v>
+      </c>
+      <c r="M28" s="9"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="1">
+        <v>4</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="8">
+        <v>45222</v>
+      </c>
+      <c r="J29" s="9"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="8">
+        <v>45225</v>
+      </c>
+      <c r="M29" s="9"/>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="1">
+        <v>3</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="8">
+        <v>45226</v>
+      </c>
+      <c r="J30" s="9"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="8">
+        <v>45228</v>
+      </c>
+      <c r="M30" s="9"/>
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="1">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="8">
+        <v>45229</v>
+      </c>
+      <c r="J31" s="9"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="8">
         <v>45230</v>
       </c>
-      <c r="M12" s="7"/>
-      <c r="N12" s="2"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="114">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:F22"/>
+    <mergeCell ref="G21:H22"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="D4:F5"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="I4:N4"/>
@@ -824,37 +1370,11 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="L6:N6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:F5"/>
-    <mergeCell ref="G4:H5"/>
-    <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="L8:N8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="B4:C5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Atualiza arquivo de especificacao de requisitos
</commit_message>
<xml_diff>
--- a/Quarto Semestre/Projeto_Integrador/Quarta Entrega/Cronograma.xlsx
+++ b/Quarto Semestre/Projeto_Integrador/Quarta Entrega/Cronograma.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richa\OneDrive\Área de Trabalho\Faculdade\Quarto Semestre\Projeto_Integrador\Quarta Entrega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3FAE12-94D1-4EAA-8656-E40D1520B8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698F7870-2EB6-4F77-B161-8ACD5F5CE922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E13B2B5E-4C2D-4D8A-B3E2-CD058EB1906D}"/>
   </bookViews>
@@ -526,11 +526,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -538,49 +580,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -899,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00196F21-3F75-4841-AD7B-9DD04B193557}">
   <dimension ref="B2:Q31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:G30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,916 +910,823 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
     <row r="4" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10" t="s">
+      <c r="K4" s="16"/>
+      <c r="L4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="10" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10" t="s">
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="2:17" ht="69" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="6" t="s">
         <v>52</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="13">
         <v>2</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="22">
+      <c r="K6" s="13"/>
+      <c r="L6" s="15">
         <v>45200</v>
       </c>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="22">
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="15">
         <v>45201</v>
       </c>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
     </row>
     <row r="7" spans="2:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="13">
         <v>3</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="22">
+      <c r="K7" s="13"/>
+      <c r="L7" s="15">
         <v>45202</v>
       </c>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="22">
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="15">
         <v>45204</v>
       </c>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="2:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="6" t="s">
         <v>57</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="13">
         <v>4</v>
       </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="22">
+      <c r="K8" s="13"/>
+      <c r="L8" s="15">
         <v>45205</v>
       </c>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="22">
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="15">
         <v>45208</v>
       </c>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-    </row>
-    <row r="9" spans="2:17" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+    </row>
+    <row r="9" spans="2:17" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="13">
+        <v>4</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="15">
+        <v>45214</v>
+      </c>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="15">
+        <v>45217</v>
+      </c>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+    </row>
+    <row r="10" spans="2:17" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="5" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E10" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="6" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J10" s="13">
         <v>5</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="22">
+      <c r="K10" s="13"/>
+      <c r="L10" s="15">
         <v>45209</v>
       </c>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="22">
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="15">
         <v>45213</v>
       </c>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-    </row>
-    <row r="10" spans="2:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" s="23">
-        <v>4</v>
-      </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="22">
-        <v>45214</v>
-      </c>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="22">
-        <v>45217</v>
-      </c>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
     </row>
     <row r="11" spans="2:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="6" t="s">
         <v>62</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11" s="13">
         <v>3</v>
       </c>
-      <c r="K11" s="23"/>
-      <c r="L11" s="22">
+      <c r="K11" s="13"/>
+      <c r="L11" s="15">
         <v>45218</v>
       </c>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="22">
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="15">
         <v>45220</v>
       </c>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
     </row>
     <row r="12" spans="2:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="23"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="6" t="s">
         <v>64</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="13">
         <v>3</v>
       </c>
-      <c r="K12" s="23"/>
-      <c r="L12" s="22">
+      <c r="K12" s="13"/>
+      <c r="L12" s="15">
         <v>45221</v>
       </c>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="22">
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="15">
         <v>45223</v>
       </c>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
     </row>
     <row r="13" spans="2:17" ht="69" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="6" t="s">
         <v>58</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J13" s="13">
         <v>2</v>
       </c>
-      <c r="K13" s="23"/>
-      <c r="L13" s="22">
+      <c r="K13" s="13"/>
+      <c r="L13" s="15">
         <v>45224</v>
       </c>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="22">
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="15">
         <v>45225</v>
       </c>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-    </row>
-    <row r="14" spans="2:17" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="s">
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="6" t="s">
         <v>76</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="13">
         <v>3</v>
       </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="22">
+      <c r="K14" s="13"/>
+      <c r="L14" s="15">
         <v>45226</v>
       </c>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="22">
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="15">
         <v>45228</v>
       </c>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
     </row>
     <row r="15" spans="2:17" ht="69" x14ac:dyDescent="0.3">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="6" t="s">
         <v>65</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J15" s="13">
         <v>2</v>
       </c>
-      <c r="K15" s="23"/>
-      <c r="L15" s="22">
+      <c r="K15" s="13"/>
+      <c r="L15" s="15">
         <v>45229</v>
       </c>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="22">
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="15">
         <v>45230</v>
       </c>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
     </row>
     <row r="16" spans="2:17" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="6" t="s">
         <v>69</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="23">
+      <c r="J16" s="13">
         <v>30</v>
       </c>
-      <c r="K16" s="23"/>
-      <c r="L16" s="22">
+      <c r="K16" s="13"/>
+      <c r="L16" s="15">
         <v>45231</v>
       </c>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="22">
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="15">
         <v>45260</v>
       </c>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
     </row>
     <row r="19" spans="2:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
     <row r="21" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10" t="s">
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="21" t="s">
+      <c r="K21" s="16"/>
+      <c r="L21" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
     </row>
     <row r="22" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="21" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21" t="s">
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
     </row>
     <row r="23" spans="2:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="14"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="6" t="s">
         <v>81</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="21">
         <v>4</v>
       </c>
-      <c r="K23" s="14"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="18">
         <v>45200</v>
       </c>
       <c r="M23" s="19"/>
-      <c r="N23" s="14"/>
+      <c r="N23" s="20"/>
       <c r="O23" s="18">
         <v>45203</v>
       </c>
       <c r="P23" s="19"/>
-      <c r="Q23" s="14"/>
+      <c r="Q23" s="20"/>
     </row>
     <row r="24" spans="2:17" ht="42" x14ac:dyDescent="0.3">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
       <c r="H24" s="6" t="s">
         <v>83</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="21">
         <v>5</v>
       </c>
-      <c r="K24" s="14"/>
+      <c r="K24" s="20"/>
       <c r="L24" s="18">
         <v>45204</v>
       </c>
       <c r="M24" s="19"/>
-      <c r="N24" s="14"/>
+      <c r="N24" s="20"/>
       <c r="O24" s="18">
         <v>45208</v>
       </c>
       <c r="P24" s="19"/>
-      <c r="Q24" s="14"/>
+      <c r="Q24" s="20"/>
     </row>
     <row r="25" spans="2:17" ht="42" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="24"/>
       <c r="H25" s="6" t="s">
         <v>85</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="J25" s="13">
+      <c r="J25" s="21">
         <v>4</v>
       </c>
-      <c r="K25" s="14"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="18">
         <v>45209</v>
       </c>
       <c r="M25" s="19"/>
-      <c r="N25" s="14"/>
+      <c r="N25" s="20"/>
       <c r="O25" s="18">
         <v>45212</v>
       </c>
       <c r="P25" s="19"/>
-      <c r="Q25" s="14"/>
+      <c r="Q25" s="20"/>
     </row>
     <row r="26" spans="2:17" ht="42" x14ac:dyDescent="0.3">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="14"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="21" t="s">
         <v>22</v>
       </c>
       <c r="F26" s="19"/>
-      <c r="G26" s="14"/>
+      <c r="G26" s="20"/>
       <c r="H26" s="8" t="s">
         <v>88</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="21">
         <v>3</v>
       </c>
-      <c r="K26" s="14"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="18">
         <v>45213</v>
       </c>
       <c r="M26" s="19"/>
-      <c r="N26" s="14"/>
+      <c r="N26" s="20"/>
       <c r="O26" s="18">
         <v>45215</v>
       </c>
       <c r="P26" s="19"/>
-      <c r="Q26" s="14"/>
+      <c r="Q26" s="20"/>
     </row>
     <row r="27" spans="2:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="14"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
       <c r="H27" s="6" t="s">
         <v>99</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="21">
         <v>3</v>
       </c>
-      <c r="K27" s="14"/>
+      <c r="K27" s="20"/>
       <c r="L27" s="18">
         <v>45216</v>
       </c>
       <c r="M27" s="19"/>
-      <c r="N27" s="14"/>
+      <c r="N27" s="20"/>
       <c r="O27" s="18">
         <v>45218</v>
       </c>
       <c r="P27" s="19"/>
-      <c r="Q27" s="14"/>
+      <c r="Q27" s="20"/>
     </row>
     <row r="28" spans="2:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="14"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="6" t="s">
         <v>98</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="21">
         <v>3</v>
       </c>
-      <c r="K28" s="14"/>
+      <c r="K28" s="20"/>
       <c r="L28" s="18">
         <v>45219</v>
       </c>
       <c r="M28" s="19"/>
-      <c r="N28" s="14"/>
+      <c r="N28" s="20"/>
       <c r="O28" s="18">
         <v>45221</v>
       </c>
       <c r="P28" s="19"/>
-      <c r="Q28" s="14"/>
+      <c r="Q28" s="20"/>
     </row>
     <row r="29" spans="2:17" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="14"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="6" t="s">
         <v>97</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="21">
         <v>4</v>
       </c>
-      <c r="K29" s="14"/>
+      <c r="K29" s="20"/>
       <c r="L29" s="18">
         <v>45222</v>
       </c>
       <c r="M29" s="19"/>
-      <c r="N29" s="14"/>
+      <c r="N29" s="20"/>
       <c r="O29" s="18">
         <v>45225</v>
       </c>
       <c r="P29" s="19"/>
-      <c r="Q29" s="14"/>
+      <c r="Q29" s="20"/>
     </row>
     <row r="30" spans="2:17" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="14"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="24"/>
       <c r="H30" s="6" t="s">
         <v>96</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="21">
         <v>3</v>
       </c>
-      <c r="K30" s="14"/>
+      <c r="K30" s="20"/>
       <c r="L30" s="18">
         <v>45226</v>
       </c>
       <c r="M30" s="19"/>
-      <c r="N30" s="14"/>
+      <c r="N30" s="20"/>
       <c r="O30" s="18">
         <v>45228</v>
       </c>
       <c r="P30" s="19"/>
-      <c r="Q30" s="14"/>
+      <c r="Q30" s="20"/>
     </row>
     <row r="31" spans="2:17" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="14"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24"/>
       <c r="H31" s="6" t="s">
         <v>95</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="21">
         <v>2</v>
       </c>
-      <c r="K31" s="14"/>
+      <c r="K31" s="20"/>
       <c r="L31" s="18">
         <v>45229</v>
       </c>
       <c r="M31" s="19"/>
-      <c r="N31" s="14"/>
+      <c r="N31" s="20"/>
       <c r="O31" s="18">
         <v>45230</v>
       </c>
       <c r="P31" s="19"/>
-      <c r="Q31" s="14"/>
+      <c r="Q31" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="120">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="L4:Q4"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="E4:G5"/>
-    <mergeCell ref="J4:K5"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="O13:Q13"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="O8:Q8"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="L10:N10"/>
     <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="L21:Q21"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="O14:Q14"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="O25:Q25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="O24:Q24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="O23:Q23"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="O28:Q28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="O27:Q27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="O26:Q26"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="O31:Q31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="O30:Q30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="O29:Q29"/>
-    <mergeCell ref="D4:D5"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H21:H22"/>
@@ -1843,9 +1750,103 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="J9:K9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="O31:Q31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="O30:Q30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="O29:Q29"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="O28:Q28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="O23:Q23"/>
+    <mergeCell ref="L21:Q21"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="L4:Q4"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="E4:G5"/>
+    <mergeCell ref="J4:K5"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>